<commit_message>
Add expiration rules for news card
</commit_message>
<xml_diff>
--- a/spreadsheets/news_archive.xlsx
+++ b/spreadsheets/news_archive.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10222"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madisonrichardson/coastwatch-wcn2/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DA4C08-4C9D-AC42-A462-903F88A83AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EA5176-4BDE-6944-A9A6-C07DA393B1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{4BBD6C59-3026-CA41-B396-04EB3E49D8C4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="209">
   <si>
     <t>Title</t>
   </si>
@@ -659,12 +659,18 @@
   </si>
   <si>
     <t>Job Opportunity: Satellite Product Modeler</t>
+  </si>
+  <si>
+    <t>Expiration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -703,7 +709,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F2D4B1-9577-ED44-8FEF-B580D6B72949}">
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,9 +1035,10 @@
     <col min="1" max="1" width="87.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,8 +1048,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1053,7 +1063,7 @@
         <v>41877</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1074,7 @@
         <v>41948</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1085,7 @@
         <v>41948</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1096,7 @@
         <v>42037</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1097,7 +1107,7 @@
         <v>42072</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1108,7 +1118,7 @@
         <v>42297</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1119,7 +1129,7 @@
         <v>42306</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1140,7 @@
         <v>42328</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>42341</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1152,7 +1162,7 @@
         <v>42412</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1163,7 +1173,7 @@
         <v>42480</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1174,7 +1184,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1196,7 +1206,7 @@
         <v>42499</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2263,7 +2273,7 @@
         <v>45897</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>205</v>
       </c>
@@ -2274,15 +2284,18 @@
         <v>45897</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>207</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" t="s">
         <v>206</v>
       </c>
       <c r="C114" s="1">
         <v>45908</v>
+      </c>
+      <c r="D114" s="2">
+        <v>46077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>